<commit_message>
Update Excel file format to have lowercase of variable.
</commit_message>
<xml_diff>
--- a/src/main/resources/BDD.xlsx
+++ b/src/main/resources/BDD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14235" windowHeight="3630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14235" windowHeight="3630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Département Suite" sheetId="9" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Ville ALL" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="G1:M9"/>
+  <oleSize ref="A4:B12"/>
 </workbook>
 </file>
 
@@ -1489,24 +1489,6 @@
     <t>variable26</t>
   </si>
   <si>
-    <t>Phrase1</t>
-  </si>
-  <si>
-    <t>Phrase2</t>
-  </si>
-  <si>
-    <t>Phrase3</t>
-  </si>
-  <si>
-    <t>Phrase4</t>
-  </si>
-  <si>
-    <t>Phrase5</t>
-  </si>
-  <si>
-    <t>Phrase6</t>
-  </si>
-  <si>
     <t>N’hésitez plus et ne perdez plus de temps</t>
   </si>
   <si>
@@ -1778,6 +1760,24 @@
   </si>
   <si>
     <t>nos opérateurs spécialisés</t>
+  </si>
+  <si>
+    <t>phrase1</t>
+  </si>
+  <si>
+    <t>phrase2</t>
+  </si>
+  <si>
+    <t>phrase3</t>
+  </si>
+  <si>
+    <t>phrase4</t>
+  </si>
+  <si>
+    <t>phrase5</t>
+  </si>
+  <si>
+    <t>phrase6</t>
   </si>
 </sst>
 </file>
@@ -2656,7 +2656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2784,7 +2784,7 @@
         <v>447</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>97</v>
@@ -2817,7 +2817,7 @@
         <v>95</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>212</v>
@@ -2835,7 +2835,7 @@
         <v>155</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>423</v>
@@ -2864,7 +2864,7 @@
         <v>448</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>197</v>
@@ -2897,7 +2897,7 @@
         <v>200</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>213</v>
@@ -2915,7 +2915,7 @@
         <v>454</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="W3" s="7" t="s">
         <v>424</v>
@@ -2944,7 +2944,7 @@
         <v>83</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>191</v>
@@ -2968,7 +2968,7 @@
         <v>453</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>140</v>
@@ -2977,7 +2977,7 @@
         <v>146</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>214</v>
@@ -2995,7 +2995,7 @@
         <v>156</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>425</v>
@@ -3042,7 +3042,7 @@
         <v>129</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>151</v>
@@ -3051,7 +3051,7 @@
         <v>147</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="Q5" s="7" t="s">
         <v>218</v>
@@ -3089,7 +3089,7 @@
         <v>85</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>192</v>
@@ -3119,7 +3119,7 @@
         <v>148</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>229</v>
@@ -3154,7 +3154,7 @@
         <v>86</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>196</v>
@@ -3176,7 +3176,7 @@
         <v>149</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="S7" s="7" t="s">
         <v>237</v>
@@ -3211,7 +3211,7 @@
         <v>87</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>464</v>
@@ -3232,7 +3232,7 @@
         <v>150</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="S8" s="7" t="s">
         <v>238</v>
@@ -3264,7 +3264,7 @@
         <v>88</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>99</v>
@@ -3282,7 +3282,7 @@
         <v>152</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="T9" s="7" t="s">
         <v>233</v>
@@ -3291,7 +3291,7 @@
         <v>161</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="Y9" s="7" t="s">
         <v>175</v>
@@ -3311,7 +3311,7 @@
         <v>89</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>195</v>
@@ -3326,7 +3326,7 @@
         <v>153</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="T10" s="7" t="s">
         <v>234</v>
@@ -3349,7 +3349,7 @@
         <v>449</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>193</v>
@@ -3385,7 +3385,7 @@
         <v>90</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>100</v>
@@ -3415,7 +3415,7 @@
         <v>91</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>451</v>
@@ -3442,7 +3442,7 @@
         <v>190</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>194</v>
@@ -3459,10 +3459,10 @@
         <v>92</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -3504,8 +3504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3520,22 +3520,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>490</v>
+        <v>581</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>491</v>
+        <v>582</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>492</v>
+        <v>583</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>493</v>
+        <v>584</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>494</v>
+        <v>585</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>495</v>
+        <v>586</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3546,10 +3546,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>241</v>
@@ -3566,10 +3566,10 @@
         <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>242</v>
@@ -3586,10 +3586,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
@@ -3604,10 +3604,10 @@
         <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
@@ -3622,7 +3622,7 @@
         <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -3638,7 +3638,7 @@
         <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -3654,7 +3654,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -4584,64 +4584,64 @@
         <v>489</v>
       </c>
       <c r="AA1" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="AG1" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>510</v>
-      </c>
-      <c r="AO1" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="AP1" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="AQ1" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="AR1" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="AS1" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="AT1" s="4" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
@@ -4673,7 +4673,7 @@
         <v>266</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>313</v>
@@ -4691,10 +4691,10 @@
         <v>413</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>253</v>
@@ -4733,7 +4733,7 @@
         <v>302</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>348</v>
@@ -4742,7 +4742,7 @@
         <v>349</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>359</v>
@@ -4763,13 +4763,13 @@
         <v>154</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="AO2" s="3" t="s">
         <v>388</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="AQ2" s="5" t="s">
         <v>424</v>
@@ -4778,7 +4778,7 @@
         <v>385</v>
       </c>
       <c r="AS2" s="6" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="AT2" s="3" t="s">
         <v>386</v>
@@ -4813,7 +4813,7 @@
         <v>264</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>314</v>
@@ -4831,7 +4831,7 @@
         <v>414</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>270</v>
@@ -4873,7 +4873,7 @@
         <v>303</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="AE3" s="3" t="s">
         <v>353</v>
@@ -4882,7 +4882,7 @@
         <v>354</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="AH3" s="3" t="s">
         <v>355</v>
@@ -4903,7 +4903,7 @@
         <v>176</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="AO3" s="3" t="s">
         <v>389</v>
@@ -4918,7 +4918,7 @@
         <v>396</v>
       </c>
       <c r="AS3" s="6" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="AT3" s="3" t="s">
         <v>399</v>
@@ -4950,7 +4950,7 @@
         <v>267</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>315</v>
@@ -4965,10 +4965,10 @@
         <v>416</v>
       </c>
       <c r="P4" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>563</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>569</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>282</v>
@@ -5004,7 +5004,7 @@
         <v>304</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="AE4" s="3" t="s">
         <v>356</v>
@@ -5028,7 +5028,7 @@
         <v>177</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="AO4" s="3" t="s">
         <v>390</v>
@@ -5040,7 +5040,7 @@
         <v>424</v>
       </c>
       <c r="AS4" s="6" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="AT4" s="3" t="s">
         <v>400</v>
@@ -5063,7 +5063,7 @@
         <v>268</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>316</v>
@@ -5078,7 +5078,7 @@
         <v>417</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>328</v>
@@ -5105,7 +5105,7 @@
         <v>305</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="AE5" s="3" t="s">
         <v>357</v>
@@ -5135,7 +5135,7 @@
         <v>425</v>
       </c>
       <c r="AS5" s="6" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="AT5" s="3" t="s">
         <v>401</v>
@@ -5155,7 +5155,7 @@
         <v>310</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>412</v>
@@ -5167,7 +5167,7 @@
         <v>419</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>410</v>
@@ -5194,7 +5194,7 @@
         <v>306</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="AE6" s="3" t="s">
         <v>358</v>
@@ -5212,7 +5212,7 @@
         <v>178</v>
       </c>
       <c r="AN6" s="3" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="AO6" s="3" t="s">
         <v>391</v>
@@ -5221,7 +5221,7 @@
         <v>426</v>
       </c>
       <c r="AS6" s="6" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="AT6" s="3" t="s">
         <v>402</v>
@@ -5244,7 +5244,7 @@
         <v>420</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>276</v>
@@ -5262,7 +5262,7 @@
         <v>307</v>
       </c>
       <c r="AD7" s="3" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="AI7" s="3" t="s">
         <v>365</v>
@@ -5277,7 +5277,7 @@
         <v>180</v>
       </c>
       <c r="AN7" s="3" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="AO7" s="3" t="s">
         <v>392</v>
@@ -5286,7 +5286,7 @@
         <v>427</v>
       </c>
       <c r="AS7" s="6" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="AT7" s="3" t="s">
         <v>403</v>
@@ -5309,7 +5309,7 @@
         <v>421</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="T8" s="3" t="s">
         <v>277</v>
@@ -5321,7 +5321,7 @@
         <v>342</v>
       </c>
       <c r="AD8" s="3" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="AI8" s="3" t="s">
         <v>366</v>
@@ -5336,7 +5336,7 @@
         <v>181</v>
       </c>
       <c r="AN8" s="3" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="AO8" s="3" t="s">
         <v>393</v>
@@ -5345,7 +5345,7 @@
         <v>428</v>
       </c>
       <c r="AS8" s="6" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="AT8" s="3" t="s">
         <v>404</v>
@@ -5365,7 +5365,7 @@
         <v>422</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>383</v>
@@ -5383,7 +5383,7 @@
         <v>182</v>
       </c>
       <c r="AN9" s="3" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="AO9" s="3" t="s">
         <v>394</v>
@@ -5392,7 +5392,7 @@
         <v>429</v>
       </c>
       <c r="AS9" s="6" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="AT9" s="3" t="s">
         <v>405</v>
@@ -5418,7 +5418,7 @@
         <v>185</v>
       </c>
       <c r="AN10" s="3" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="AQ10" s="5" t="s">
         <v>430</v>
@@ -5438,7 +5438,7 @@
         <v>183</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="AT11" s="3" t="s">
         <v>407</v>
@@ -5452,7 +5452,7 @@
         <v>184</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="AT12" s="3" t="s">
         <v>408</v>
@@ -5466,7 +5466,7 @@
         <v>186</v>
       </c>
       <c r="AN13" s="3" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="AO13" s="6"/>
       <c r="AT13" s="3" t="s">
@@ -5475,13 +5475,13 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AN14" s="3" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="AO14" s="6"/>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AN15" s="3" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="AO15" s="6"/>
     </row>

</xml_diff>

<commit_message>
Add new Selenium tests
</commit_message>
<xml_diff>
--- a/src/main/resources/BDD.xlsx
+++ b/src/main/resources/BDD.xlsx
@@ -3,21 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khoa\git\urgencemedecin\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14235" windowHeight="3630" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14235" windowHeight="3630"/>
   </bookViews>
   <sheets>
-    <sheet name="Département Suite" sheetId="9" r:id="rId1"/>
-    <sheet name="Ville Accroche" sheetId="10" r:id="rId2"/>
-    <sheet name="Ville ALL" sheetId="11" r:id="rId3"/>
+    <sheet name="Département Accroche" sheetId="12" r:id="rId1"/>
+    <sheet name="Département Suite" sheetId="9" r:id="rId2"/>
+    <sheet name="Ville Accroche" sheetId="10" r:id="rId3"/>
+    <sheet name="Ville ALL" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A4:B12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="641">
   <si>
     <t>La page de cet annuaire vous permettra de chercher</t>
   </si>
@@ -1778,6 +1783,168 @@
   </si>
   <si>
     <t>phrase6</t>
+  </si>
+  <si>
+    <t>Grâce à notre site, vous pouvez trouver rapidement</t>
+  </si>
+  <si>
+    <t>dès que vous en ressentez la nécessité</t>
+  </si>
+  <si>
+    <t>Découvrez les solutions grâce à nos conseillers afin de trouver</t>
+  </si>
+  <si>
+    <t>dès que le besoin se fait ressentir</t>
+  </si>
+  <si>
+    <t>Toutes nos équipes vous accompagnent afin de trouver</t>
+  </si>
+  <si>
+    <t>à tout moment de la journée</t>
+  </si>
+  <si>
+    <t>Tous nos consultants spécialisées vous aident à trouver</t>
+  </si>
+  <si>
+    <t>lorsque vous avez besoin d'une consultation</t>
+  </si>
+  <si>
+    <t>Tous nos conseillers vous accompagnent afin de récupérer et trouver</t>
+  </si>
+  <si>
+    <t>si vous avez un besoin médical en dehors des horaires habituels</t>
+  </si>
+  <si>
+    <t>Grâce à nos équipes de téléconseillers, trouvez facilement</t>
+  </si>
+  <si>
+    <t>dès que le besoin demande un conseil médical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nos consultants en ligne, vous aident pour trouver rapidement </t>
+  </si>
+  <si>
+    <t>dès que vous ressentez l'envie de parler à un spécialiste</t>
+  </si>
+  <si>
+    <t>Une question médicale, besoin d'un conseil nos équipes vous trouvent</t>
+  </si>
+  <si>
+    <t>dés que le moment vous parait opportun</t>
+  </si>
+  <si>
+    <t>Un besoin urgent, une demande médicale, nous vous aidons à trouver</t>
+  </si>
+  <si>
+    <t>lorsque vous pensez avoir besoin d'un conseil médical</t>
+  </si>
+  <si>
+    <t>Notre offre de renseignements, vous permet facilement de trouver</t>
+  </si>
+  <si>
+    <t>si vous pensez que c'est le moment d'avoir un conseil d'un spécialiste</t>
+  </si>
+  <si>
+    <t>Notre offre de renseignements, vous permet rapidement de récupérer</t>
+  </si>
+  <si>
+    <t>dès qu'un besoin urgent se fait ressentir</t>
+  </si>
+  <si>
+    <t>Avec notre site internet, vous pouvez récupérer facilement</t>
+  </si>
+  <si>
+    <t>dès lors que le besoin d'un conseil médical se fait ressentir</t>
+  </si>
+  <si>
+    <t>Découvrez les différentes solutions afin de trouver rapidement</t>
+  </si>
+  <si>
+    <t>dès que vous en éprouvez le besoin</t>
+  </si>
+  <si>
+    <t>Nos équipes vous accompagnent dans la recherche afin de trouver</t>
+  </si>
+  <si>
+    <t>qui pourra répondre à vos demandes médicales</t>
+  </si>
+  <si>
+    <t>qui pourra vous aider dans vos demandes médicales</t>
+  </si>
+  <si>
+    <t>En vous connectant à notre page, vous trouverez facilement comment récupérer</t>
+  </si>
+  <si>
+    <t>qui pourra vous rassurer sur vos problèmes d'ordre médicaux</t>
+  </si>
+  <si>
+    <t>Bonjour, vous voilà bien sur l'annuaire</t>
+  </si>
+  <si>
+    <t>Toutes nos équipes spécialisées vous aident afin de trouver</t>
+  </si>
+  <si>
+    <t>qui pourra vous rassurer sur vos symptômes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grâce à nos téléconseillers, découvrez comment trouver </t>
+  </si>
+  <si>
+    <t>qui pourra analyser vos symptômes</t>
+  </si>
+  <si>
+    <t>Grâce à nos équipes de téléconseillers, découvrez comment récupérer</t>
+  </si>
+  <si>
+    <t>qui vous aidera afin d'analyser vos symptômes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grâce à nos consultants téléconseillers, découvrez comment chercher et trouver </t>
+  </si>
+  <si>
+    <t>à tout moment de la semaine</t>
+  </si>
+  <si>
+    <t>Cette page web vous offre un service qui vous permettra facilement de trouver</t>
+  </si>
+  <si>
+    <t>qui sera à même de répondre à toutes vos questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette page internet vous donne accès à un service afin de récupérer </t>
+  </si>
+  <si>
+    <t>qui sera capable de répondre à vos questions et analyser vos symptômes</t>
+  </si>
+  <si>
+    <t>Cette page web vous donne un service de mise en relation afin de trouver</t>
+  </si>
+  <si>
+    <t>qui sera dans la capacité de vous aider et répondre à vos questions médicales</t>
+  </si>
+  <si>
+    <t>En passant par notre site internet, nous vous aidons rapidement afin de trouver</t>
+  </si>
+  <si>
+    <t>qui vous répondra sur les questions et symptômes que vous ressentez</t>
+  </si>
+  <si>
+    <t>qui écoutera les symptômes que vous ressentez</t>
+  </si>
+  <si>
+    <t>qui pourra vous donner des élements de réponses sur vos symptômes</t>
+  </si>
+  <si>
+    <t>qui vous dira ce qu'il faut faire selon votre situation médicale</t>
+  </si>
+  <si>
+    <t>qui vous écoutera afin de trouver une solution à vos problèmes</t>
+  </si>
+  <si>
+    <t>qui donnera des élements de réponses à vos questions</t>
+  </si>
+  <si>
+    <t>qui sera à l'écoute de vos demandes afin de trouver une solution</t>
   </si>
 </sst>
 </file>
@@ -2654,9 +2821,322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B3" t="s">
+        <v>589</v>
+      </c>
+      <c r="C3" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>593</v>
+      </c>
+      <c r="C5" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>595</v>
+      </c>
+      <c r="C6" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>597</v>
+      </c>
+      <c r="C7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>599</v>
+      </c>
+      <c r="C8" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>432</v>
+      </c>
+      <c r="B9" t="s">
+        <v>601</v>
+      </c>
+      <c r="C9" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>433</v>
+      </c>
+      <c r="B10" t="s">
+        <v>603</v>
+      </c>
+      <c r="C10" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>468</v>
+      </c>
+      <c r="B11" t="s">
+        <v>605</v>
+      </c>
+      <c r="C11" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>434</v>
+      </c>
+      <c r="B12" t="s">
+        <v>607</v>
+      </c>
+      <c r="C12" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>435</v>
+      </c>
+      <c r="B13" t="s">
+        <v>609</v>
+      </c>
+      <c r="C13" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>611</v>
+      </c>
+      <c r="C14" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>613</v>
+      </c>
+      <c r="C15" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>609</v>
+      </c>
+      <c r="C16" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>618</v>
+      </c>
+      <c r="B17" t="s">
+        <v>616</v>
+      </c>
+      <c r="C17" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>619</v>
+      </c>
+      <c r="C18" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>621</v>
+      </c>
+      <c r="C19" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>623</v>
+      </c>
+      <c r="C20" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" t="s">
+        <v>625</v>
+      </c>
+      <c r="C21" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>627</v>
+      </c>
+      <c r="C22" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>629</v>
+      </c>
+      <c r="C23" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>631</v>
+      </c>
+      <c r="C24" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>633</v>
+      </c>
+      <c r="C25" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>640</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3500,12 +3980,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4443,7 +4923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV24"/>
   <sheetViews>

</xml_diff>